<commit_message>
Added lineup picture to results
</commit_message>
<xml_diff>
--- a/Player Stats.xlsx
+++ b/Player Stats.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet3" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Players" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Results" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet2!$A$1:$J$20</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Players!$A$1:$J$21</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -46,61 +46,64 @@
     <t>Win Percentage</t>
   </si>
   <si>
-    <t>Gavin</t>
-  </si>
-  <si>
-    <t>Kieran</t>
-  </si>
-  <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>Chris</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Phil</t>
-  </si>
-  <si>
-    <t>Dida</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
-    <t>Ollie</t>
-  </si>
-  <si>
-    <t>Ferdi</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Bernard</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Rik</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Will</t>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Player 3</t>
+  </si>
+  <si>
+    <t>Player 4</t>
+  </si>
+  <si>
+    <t>Player 5</t>
+  </si>
+  <si>
+    <t>Player 6</t>
+  </si>
+  <si>
+    <t>Player 7</t>
+  </si>
+  <si>
+    <t>Player 8</t>
+  </si>
+  <si>
+    <t>Player 9</t>
+  </si>
+  <si>
+    <t>Player 10</t>
+  </si>
+  <si>
+    <t>Player 11</t>
+  </si>
+  <si>
+    <t>Player 12</t>
+  </si>
+  <si>
+    <t>Player 13</t>
+  </si>
+  <si>
+    <t>Player 14</t>
+  </si>
+  <si>
+    <t>Player 15</t>
+  </si>
+  <si>
+    <t>Player 16</t>
+  </si>
+  <si>
+    <t>Player 17</t>
+  </si>
+  <si>
+    <t>Player 18</t>
+  </si>
+  <si>
+    <t>Player 19</t>
+  </si>
+  <si>
+    <t>Player 20</t>
   </si>
   <si>
     <t>Date</t>
@@ -146,21 +149,6 @@
   </si>
   <si>
     <t>Team B Player 5</t>
-  </si>
-  <si>
-    <t>"2021-01-04"</t>
-  </si>
-  <si>
-    <t>Rich</t>
-  </si>
-  <si>
-    <t>"2021-01-11"</t>
-  </si>
-  <si>
-    <t>"2021-01-13"</t>
-  </si>
-  <si>
-    <t>"2021-01-20"</t>
   </si>
 </sst>
 </file>
@@ -178,11 +166,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,28 +188,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -494,24 +475,24 @@
         <v>19.0</v>
       </c>
       <c r="G2" s="3">
-        <f t="shared" ref="G2:G20" si="1">SUM(B2:F2)+H2</f>
+        <f t="shared" ref="G2:G21" si="1">SUM(B2:F2)+H2</f>
         <v>81</v>
       </c>
       <c r="H2" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A2)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A2)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A2)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A2)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I2" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J987 = $A2)*(Sheet3!$B2:$B987&lt;Sheet3!$C2:$C987)))+(SUMPRODUCT((Sheet3!$K2:$O987 = $A2)*(Sheet3!$B2:$B987&gt;Sheet3!$C2:$C987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J974 = $A2)*(Results!$B2:$B974&lt;Results!$C2:$C974)))+(SUMPRODUCT((Results!$K2:$O974 = $A2)*(Results!$B2:$B974&gt;Results!$C2:$C974)))</f>
         <v>0</v>
       </c>
       <c r="J2" s="4">
-        <f t="shared" ref="J2:J20" si="2">IFERROR(H2/(H2+I2),0)</f>
+        <f t="shared" ref="J2:J21" si="2">IFERROR(H2/(H2+I2),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1">
@@ -534,11 +515,11 @@
         <v>81</v>
       </c>
       <c r="H3" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A3)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A3)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A3)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A3)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I3" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F11:$J1008 = $A3)*(Sheet3!$B11:$B1008&lt;Sheet3!$C11:$C1008)))+(SUMPRODUCT((Sheet3!$K11:$O1008 = $A3)*(Sheet3!$B11:$B1008&gt;Sheet3!$C11:$C1008)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J995 = $A3)*(Results!$B2:$B995&lt;Results!$C2:$C995)))+(SUMPRODUCT((Results!$K2:$O995 = $A3)*(Results!$B2:$B995&gt;Results!$C2:$C995)))</f>
         <v>0</v>
       </c>
       <c r="J3" s="4">
@@ -547,7 +528,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1">
@@ -570,11 +551,11 @@
         <v>80</v>
       </c>
       <c r="H4" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A4)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A4)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A4)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A4)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I4" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J989 = $A4)*(Sheet3!$B2:$B989&lt;Sheet3!$C2:$C989)))+(SUMPRODUCT((Sheet3!$K2:$O989 = $A4)*(Sheet3!$B2:$B989&gt;Sheet3!$C2:$C989)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J976 = $A4)*(Results!$B2:$B976&lt;Results!$C2:$C976)))+(SUMPRODUCT((Results!$K2:$O976 = $A4)*(Results!$B2:$B976&gt;Results!$C2:$C976)))</f>
         <v>0</v>
       </c>
       <c r="J4" s="4">
@@ -583,7 +564,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1">
@@ -606,11 +587,11 @@
         <v>79</v>
       </c>
       <c r="H5" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A5)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A5)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A5)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A5)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I5" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J990 = $A5)*(Sheet3!$B2:$B990&lt;Sheet3!$C2:$C990)))+(SUMPRODUCT((Sheet3!$K2:$O990 = $A5)*(Sheet3!$B2:$B990&gt;Sheet3!$C2:$C990)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J977 = $A5)*(Results!$B2:$B977&lt;Results!$C2:$C977)))+(SUMPRODUCT((Results!$K2:$O977 = $A5)*(Results!$B2:$B977&gt;Results!$C2:$C977)))</f>
         <v>0</v>
       </c>
       <c r="J5" s="4">
@@ -642,11 +623,11 @@
         <v>79</v>
       </c>
       <c r="H6" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A6)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A6)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A6)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A6)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I6" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J991 = $A6)*(Sheet3!$B2:$B991&lt;Sheet3!$C2:$C991)))+(SUMPRODUCT((Sheet3!$K2:$O991 = $A6)*(Sheet3!$B2:$B991&gt;Sheet3!$C2:$C991)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J978 = $A6)*(Results!$B2:$B978&lt;Results!$C2:$C978)))+(SUMPRODUCT((Results!$K2:$O978 = $A6)*(Results!$B2:$B978&gt;Results!$C2:$C978)))</f>
         <v>0</v>
       </c>
       <c r="J6" s="4">
@@ -678,11 +659,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A7)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A7)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A7)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A7)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I7" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J992 = $A7)*(Sheet3!$B2:$B992&lt;Sheet3!$C2:$C992)))+(SUMPRODUCT((Sheet3!$K2:$O992 = $A7)*(Sheet3!$B2:$B992&gt;Sheet3!$C2:$C992)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J979 = $A7)*(Results!$B2:$B979&lt;Results!$C2:$C979)))+(SUMPRODUCT((Results!$K2:$O979 = $A7)*(Results!$B2:$B979&gt;Results!$C2:$C979)))</f>
         <v>0</v>
       </c>
       <c r="J7" s="4">
@@ -691,7 +672,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1">
@@ -714,11 +695,11 @@
         <v>78</v>
       </c>
       <c r="H8" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A8)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A8)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A8)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A8)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I8" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J988 = $A8)*(Sheet3!$B2:$B988&lt;Sheet3!$C2:$C988)))+(SUMPRODUCT((Sheet3!$K2:$O988 = $A8)*(Sheet3!$B2:$B988&gt;Sheet3!$C2:$C988)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J975 = $A8)*(Results!$B2:$B975&lt;Results!$C2:$C975)))+(SUMPRODUCT((Results!$K2:$O975 = $A8)*(Results!$B2:$B975&gt;Results!$C2:$C975)))</f>
         <v>0</v>
       </c>
       <c r="J8" s="4">
@@ -750,11 +731,11 @@
         <v>78</v>
       </c>
       <c r="H9" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A9)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A9)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A9)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A9)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I9" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J994 = $A9)*(Sheet3!$B2:$B994&lt;Sheet3!$C2:$C994)))+(SUMPRODUCT((Sheet3!$K2:$O994 = $A9)*(Sheet3!$B2:$B994&gt;Sheet3!$C2:$C994)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J981 = $A9)*(Results!$B2:$B981&lt;Results!$C2:$C981)))+(SUMPRODUCT((Results!$K2:$O981 = $A9)*(Results!$B2:$B981&gt;Results!$C2:$C981)))</f>
         <v>0</v>
       </c>
       <c r="J9" s="4">
@@ -763,7 +744,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1">
@@ -786,11 +767,11 @@
         <v>77</v>
       </c>
       <c r="H10" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A10)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A10)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A10)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A10)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I10" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J993 = $A10)*(Sheet3!$B2:$B993&lt;Sheet3!$C2:$C993)))+(SUMPRODUCT((Sheet3!$K2:$O993 = $A10)*(Sheet3!$B2:$B993&gt;Sheet3!$C2:$C993)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J980 = $A10)*(Results!$B2:$B980&lt;Results!$C2:$C980)))+(SUMPRODUCT((Results!$K2:$O980 = $A10)*(Results!$B2:$B980&gt;Results!$C2:$C980)))</f>
         <v>0</v>
       </c>
       <c r="J10" s="4">
@@ -822,11 +803,11 @@
         <v>71</v>
       </c>
       <c r="H11" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A11)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A11)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A11)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A11)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I11" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J996 = $A11)*(Sheet3!$B2:$B996&lt;Sheet3!$C2:$C996)))+(SUMPRODUCT((Sheet3!$K2:$O996 = $A11)*(Sheet3!$B2:$B996&gt;Sheet3!$C2:$C996)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J983 = $A11)*(Results!$B2:$B983&lt;Results!$C2:$C983)))+(SUMPRODUCT((Results!$K2:$O983 = $A11)*(Results!$B2:$B983&gt;Results!$C2:$C983)))</f>
         <v>0</v>
       </c>
       <c r="J11" s="4">
@@ -858,11 +839,11 @@
         <v>71</v>
       </c>
       <c r="H12" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A12)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A12)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A12)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A12)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I12" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J995 = $A12)*(Sheet3!$B2:$B995&lt;Sheet3!$C2:$C995)))+(SUMPRODUCT((Sheet3!$K2:$O995 = $A12)*(Sheet3!$B2:$B995&gt;Sheet3!$C2:$C995)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J982 = $A12)*(Results!$B2:$B982&lt;Results!$C2:$C982)))+(SUMPRODUCT((Results!$K2:$O982 = $A12)*(Results!$B2:$B982&gt;Results!$C2:$C982)))</f>
         <v>0</v>
       </c>
       <c r="J12" s="4">
@@ -871,7 +852,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="1">
@@ -894,11 +875,11 @@
         <v>69</v>
       </c>
       <c r="H13" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A13)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A13)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A13)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A13)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I13" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F3:$J998 = $A13)*(Sheet3!$B3:$B998&lt;Sheet3!$C3:$C998)))+(SUMPRODUCT((Sheet3!$K3:$O998 = $A13)*(Sheet3!$B3:$B998&gt;Sheet3!$C3:$C998)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J985 = $A13)*(Results!$B2:$B985&lt;Results!$C2:$C985)))+(SUMPRODUCT((Results!$K2:$O985 = $A13)*(Results!$B2:$B985&gt;Results!$C2:$C985)))</f>
         <v>0</v>
       </c>
       <c r="J13" s="4">
@@ -930,11 +911,11 @@
         <v>69</v>
       </c>
       <c r="H14" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A14)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A14)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A14)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A14)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I14" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F2:$J997 = $A14)*(Sheet3!$B2:$B997&lt;Sheet3!$C2:$C997)))+(SUMPRODUCT((Sheet3!$K2:$O997 = $A14)*(Sheet3!$B2:$B997&gt;Sheet3!$C2:$C997)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J984 = $A14)*(Results!$B2:$B984&lt;Results!$C2:$C984)))+(SUMPRODUCT((Results!$K2:$O984 = $A14)*(Results!$B2:$B984&gt;Results!$C2:$C984)))</f>
         <v>0</v>
       </c>
       <c r="J14" s="4">
@@ -966,11 +947,11 @@
         <v>68</v>
       </c>
       <c r="H15" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A15)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A15)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A15)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A15)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I15" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F4:$J999 = $A15)*(Sheet3!$B4:$B999&lt;Sheet3!$C4:$C999)))+(SUMPRODUCT((Sheet3!$K4:$O999 = $A15)*(Sheet3!$B4:$B999&gt;Sheet3!$C4:$C999)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J986 = $A15)*(Results!$B2:$B986&lt;Results!$C2:$C986)))+(SUMPRODUCT((Results!$K2:$O986 = $A15)*(Results!$B2:$B986&gt;Results!$C2:$C986)))</f>
         <v>0</v>
       </c>
       <c r="J15" s="4">
@@ -1002,11 +983,11 @@
         <v>66</v>
       </c>
       <c r="H16" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A16)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A16)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A16)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A16)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I16" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F5:$J1000 = $A16)*(Sheet3!$B5:$B1000&lt;Sheet3!$C5:$C1000)))+(SUMPRODUCT((Sheet3!$K5:$O1000 = $A16)*(Sheet3!$B5:$B1000&gt;Sheet3!$C5:$C1000)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J987 = $A16)*(Results!$B2:$B987&lt;Results!$C2:$C987)))+(SUMPRODUCT((Results!$K2:$O987 = $A16)*(Results!$B2:$B987&gt;Results!$C2:$C987)))</f>
         <v>0</v>
       </c>
       <c r="J16" s="4">
@@ -1019,30 +1000,30 @@
         <v>25</v>
       </c>
       <c r="B17" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="D17" s="1">
         <v>14.0</v>
       </c>
-      <c r="C17" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>10.0</v>
-      </c>
       <c r="E17" s="1">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="F17" s="1">
-        <v>9.0</v>
+        <v>13.0</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="H17" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A17)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A17)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A17)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A17)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I17" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F5:$J1001 = $A17)*(Sheet3!$B5:$B1001&lt;Sheet3!$C5:$C1001)))+(SUMPRODUCT((Sheet3!$K5:$O1001 = $A17)*(Sheet3!$B5:$B1001&gt;Sheet3!$C5:$C1001)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J988 = $A17)*(Results!$B2:$B988&lt;Results!$C2:$C988)))+(SUMPRODUCT((Results!$K2:$O988 = $A17)*(Results!$B2:$B988&gt;Results!$C2:$C988)))</f>
         <v>0</v>
       </c>
       <c r="J17" s="4">
@@ -1055,30 +1036,30 @@
         <v>26</v>
       </c>
       <c r="B18" s="1">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="C18" s="1">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="D18" s="1">
         <v>10.0</v>
       </c>
       <c r="E18" s="1">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="F18" s="1">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H18" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A18)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A18)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A18)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A18)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I18" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F5:$J1002 = $A18)*(Sheet3!$B5:$B1002&lt;Sheet3!$C5:$C1002)))+(SUMPRODUCT((Sheet3!$K5:$O1002 = $A18)*(Sheet3!$B5:$B1002&gt;Sheet3!$C5:$C1002)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J988 = $A18)*(Results!$B2:$B988&lt;Results!$C2:$C988)))+(SUMPRODUCT((Results!$K2:$O988 = $A18)*(Results!$B2:$B988&gt;Results!$C2:$C988)))</f>
         <v>0</v>
       </c>
       <c r="J18" s="4">
@@ -1091,49 +1072,49 @@
         <v>27</v>
       </c>
       <c r="B19" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="E19" s="1">
         <v>11.0</v>
       </c>
-      <c r="C19" s="1">
+      <c r="F19" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="H19" s="3">
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A19)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A19)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <f>SUM(SUMPRODUCT((Results!$F2:$J989 = $A19)*(Results!$B2:$B989&lt;Results!$C2:$C989)))+(SUMPRODUCT((Results!$K2:$O989 = $A19)*(Results!$B2:$B989&gt;Results!$C2:$C989)))</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
         <v>11.0</v>
       </c>
-      <c r="D19" s="1">
+      <c r="C20" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="D20" s="1">
         <v>9.0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="H19" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A19)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A19)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F6:$J1003 = $A19)*(Sheet3!$B6:$B1003&lt;Sheet3!$C6:$C1003)))+(SUMPRODUCT((Sheet3!$K6:$O1003 = $A19)*(Sheet3!$B6:$B1003&gt;Sheet3!$C6:$C1003)))</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>13.0</v>
       </c>
       <c r="E20" s="1">
         <v>9.0</v>
@@ -1146,11 +1127,11 @@
         <v>47</v>
       </c>
       <c r="H20" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F$2:$J$987 = $A20)*(Sheet3!$B$2:$B$987&gt;Sheet3!$C$2:$C$987)))+(SUMPRODUCT((Sheet3!$K$2:$O$987 = $A20)*(Sheet3!$B$2:$B$987&lt;Sheet3!$C$2:$C$987)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A20)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A20)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
         <v>0</v>
       </c>
       <c r="I20" s="3">
-        <f>SUM(SUMPRODUCT((Sheet3!$F7:$J1004 = $A20)*(Sheet3!$B7:$B1004&lt;Sheet3!$C7:$C1004)))+(SUMPRODUCT((Sheet3!$K7:$O1004 = $A20)*(Sheet3!$B7:$B1004&gt;Sheet3!$C7:$C1004)))</f>
+        <f>SUM(SUMPRODUCT((Results!$F2:$J990 = $A20)*(Results!$B2:$B990&lt;Results!$C2:$C990)))+(SUMPRODUCT((Results!$K2:$O990 = $A20)*(Results!$B2:$B990&gt;Results!$C2:$C990)))</f>
         <v>0</v>
       </c>
       <c r="J20" s="4">
@@ -1158,10 +1139,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="H21" s="3">
+        <f>SUM(SUMPRODUCT((Results!$F$2:$J$974 = $A21)*(Results!$B$2:$B$974&gt;Results!$C$2:$C$974)))+(SUMPRODUCT((Results!$K$2:$O$974 = $A21)*(Results!$B$2:$B$974&lt;Results!$C$2:$C$974)))</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <f>SUM(SUMPRODUCT((Results!$F2:$J991 = $A21)*(Results!$B2:$B991&lt;Results!$C2:$C991)))+(SUMPRODUCT((Results!$K2:$O991 = $A21)*(Results!$B2:$B991&gt;Results!$C2:$C991)))</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$20">
-    <sortState ref="A1:J20">
-      <sortCondition descending="1" ref="G1:G20"/>
+  <autoFilter ref="$A$1:$J$21">
+    <sortState ref="A1:J21">
+      <sortCondition descending="1" ref="G1:G21"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>
@@ -1187,238 +1204,50 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="8">
-        <v>420.0</v>
-      </c>
-      <c r="E2" s="8">
-        <v>376.0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>375.0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>375.0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>416.0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>413.0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>357.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>350.0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>